<commit_message>
Added review date to test result summary.
</commit_message>
<xml_diff>
--- a/documentation/alphaTestRound/voltaicSparrow_alphaTestSummary_03232023.xlsx
+++ b/documentation/alphaTestRound/voltaicSparrow_alphaTestSummary_03232023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2023\CIS4914\modules\3_softwareImplementation\rawTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2023\CIS4914\VoltaicSparrow\documentation\alphaTestRound\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484AAB72-55C5-40A4-8CBF-BB6E1182DA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CFBC0A-4659-450E-849B-67BEE00286D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Project Name</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>0325/2023</t>
   </si>
 </sst>
 </file>
@@ -609,7 +612,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +687,9 @@
         <v>3</v>
       </c>
       <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="1"/>

</xml_diff>